<commit_message>
JSON for wonders finished
</commit_message>
<xml_diff>
--- a/resources/Wonders.xlsx
+++ b/resources/Wonders.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\merreltc\Documents\GitHub\Silver_Falcons_Seven_Wonders\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="985"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -22,249 +26,231 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="69">
   <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Side</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Level Priority</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Effect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frequency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Effect 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Colossus of Rhodes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 Lumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 Victory Points</t>
-  </si>
-  <si>
-    <t xml:space="preserve">End of Game</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resource</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 Clay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 Conflict Tokens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Once</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 Ore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 Victory Points</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 Stone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Conflict Token&amp;3 Coins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Conflict Token&amp;4 Coins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 Victory Points</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Lighthouse of Alexandria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 Stone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 Ore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Clay/Ore/Lumber/Stone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Every Turn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 Glass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 Clay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Glass/Loom/Press</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Temple of Artemis in Ephesus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9 Coins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Press</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 Press</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 Coins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 Victory Points</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Press&amp;Loom&amp;Glass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 Victory Points</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Hanging Gardens of Babylon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 Lumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Tablet/Protractor/Wheel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 Clay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Loom&amp;Clay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Glass&amp;2 Lumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Play seventh card</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sixth Turn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Press&amp;3 Clay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Statue of Zeus in Olympia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Free structure building</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Once per Age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Coin Raw Material Trade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Loom&amp;2 Ore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Copy 1 Neighbors Guild Card</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Mausoleum of Halicarnassus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 Ore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pick from discard and build free</t>
-  </si>
-  <si>
-    <t xml:space="preserve">End of Turn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Loom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 Loom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Victory Point</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Pyramids of Giza</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 Stone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Press&amp;4 Stone</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Side</t>
+  </si>
+  <si>
+    <t>Level Priority</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Effect</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Effect 2</t>
+  </si>
+  <si>
+    <t>The Colossus of Rhodes</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>2 Lumber</t>
+  </si>
+  <si>
+    <t>3 Victory Points</t>
+  </si>
+  <si>
+    <t>End of Game</t>
+  </si>
+  <si>
+    <t>Resource</t>
+  </si>
+  <si>
+    <t>3 Clay</t>
+  </si>
+  <si>
+    <t>2 Conflict Tokens</t>
+  </si>
+  <si>
+    <t>Once</t>
+  </si>
+  <si>
+    <t>Ore</t>
+  </si>
+  <si>
+    <t>4 Ore</t>
+  </si>
+  <si>
+    <t>7 Victory Points</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>3 Stone</t>
+  </si>
+  <si>
+    <t>1 Conflict Token&amp;3 Coins</t>
+  </si>
+  <si>
+    <t>1 Conflict Token&amp;4 Coins</t>
+  </si>
+  <si>
+    <t>4 Victory Points</t>
+  </si>
+  <si>
+    <t>The Lighthouse of Alexandria</t>
+  </si>
+  <si>
+    <t>2 Stone</t>
+  </si>
+  <si>
+    <t>2 Ore</t>
+  </si>
+  <si>
+    <t>1 Clay/Ore/Lumber/Stone</t>
+  </si>
+  <si>
+    <t>Every Turn</t>
+  </si>
+  <si>
+    <t>Glass</t>
+  </si>
+  <si>
+    <t>2 Glass</t>
+  </si>
+  <si>
+    <t>2 Clay</t>
+  </si>
+  <si>
+    <t>1 Glass/Loom/Press</t>
+  </si>
+  <si>
+    <t>The Temple of Artemis in Ephesus</t>
+  </si>
+  <si>
+    <t>9 Coins</t>
+  </si>
+  <si>
+    <t>Press</t>
+  </si>
+  <si>
+    <t>2 Press</t>
+  </si>
+  <si>
+    <t>4 Coins</t>
+  </si>
+  <si>
+    <t>2 Victory Points</t>
+  </si>
+  <si>
+    <t>1 Press&amp;Loom&amp;Glass</t>
+  </si>
+  <si>
+    <t>5 Victory Points</t>
+  </si>
+  <si>
+    <t>The Hanging Gardens of Babylon</t>
+  </si>
+  <si>
+    <t>3 Lumber</t>
+  </si>
+  <si>
+    <t>1 Tablet/Protractor/Wheel</t>
+  </si>
+  <si>
+    <t>Clay</t>
+  </si>
+  <si>
+    <t>4 Clay</t>
+  </si>
+  <si>
+    <t>1 Loom&amp;Clay</t>
+  </si>
+  <si>
+    <t>1 Glass&amp;2 Lumber</t>
+  </si>
+  <si>
+    <t>Play seventh card</t>
+  </si>
+  <si>
+    <t>Sixth Turn</t>
+  </si>
+  <si>
+    <t>1 Press&amp;3 Clay</t>
+  </si>
+  <si>
+    <t>The Statue of Zeus in Olympia</t>
+  </si>
+  <si>
+    <t>Free structure building</t>
+  </si>
+  <si>
+    <t>Once per Age</t>
+  </si>
+  <si>
+    <t>Lumber</t>
+  </si>
+  <si>
+    <t>1 Coin Raw Material Trade</t>
+  </si>
+  <si>
+    <t>1 Loom&amp;2 Ore</t>
+  </si>
+  <si>
+    <t>Copy 1 Neighbors Guild Card</t>
+  </si>
+  <si>
+    <t>The Mausoleum of Halicarnassus</t>
+  </si>
+  <si>
+    <t>3 Ore</t>
+  </si>
+  <si>
+    <t>Pick from discard and build free</t>
+  </si>
+  <si>
+    <t>End of Turn</t>
+  </si>
+  <si>
+    <t>Loom</t>
+  </si>
+  <si>
+    <t>2 Loom</t>
+  </si>
+  <si>
+    <t>1 Victory Point</t>
+  </si>
+  <si>
+    <t>The Pyramids of Giza</t>
+  </si>
+  <si>
+    <t>Stone</t>
+  </si>
+  <si>
+    <t>4 Stone</t>
+  </si>
+  <si>
+    <t>1 Press&amp;4 Stone</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="18"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <i val="true"/>
+      <i/>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -290,7 +276,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -298,73 +284,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -423,36 +374,310 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="1:49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK49"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E46" activeCellId="0" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="D22" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D22" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="43.3520408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.9642857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="25.5561224489796"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="41.4489795918367"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="20.7448979591837"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="38.9030612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.8163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="11.5204081632653"/>
+    <col min="1" max="1" width="43.33203125" style="1"/>
+    <col min="2" max="2" width="11.5546875" style="1"/>
+    <col min="3" max="3" width="23" style="1"/>
+    <col min="4" max="4" width="25.5546875" style="2"/>
+    <col min="5" max="5" width="41.44140625" style="2"/>
+    <col min="6" max="6" width="20.77734375" style="2"/>
+    <col min="7" max="7" width="38.88671875" style="1"/>
+    <col min="8" max="8" width="19.77734375" style="1"/>
+    <col min="9" max="1025" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:1024" s="3" customFormat="1" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -479,14 +704,14 @@
       </c>
       <c r="AMJ1" s="4"/>
     </row>
-    <row r="2" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:1024" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="6" t="n">
+      <c r="C2" s="6">
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
@@ -500,14 +725,14 @@
       </c>
       <c r="AMJ2" s="1"/>
     </row>
-    <row r="3" s="6" customFormat="true" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:1024" s="6" customFormat="1" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="6" t="n">
+      <c r="C3" s="6">
         <v>2</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -521,14 +746,14 @@
       </c>
       <c r="AMJ3" s="1"/>
     </row>
-    <row r="4" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:1024" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="6" t="n">
+      <c r="C4" s="6">
         <v>3</v>
       </c>
       <c r="D4" s="7" t="s">
@@ -542,12 +767,12 @@
       </c>
       <c r="AMJ4" s="1"/>
     </row>
-    <row r="5" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:1024" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="B5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="6" t="n">
+      <c r="C5" s="6">
         <v>1</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -567,12 +792,12 @@
       </c>
       <c r="AMJ5" s="1"/>
     </row>
-    <row r="6" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:1024" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
       <c r="B6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="6" t="n">
+      <c r="C6" s="6">
         <v>2</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -592,7 +817,7 @@
       </c>
       <c r="AMJ6" s="1"/>
     </row>
-    <row r="7" s="3" customFormat="true" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:1024" s="3" customFormat="1" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
@@ -610,14 +835,14 @@
       </c>
       <c r="AMJ7" s="4"/>
     </row>
-    <row r="8" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:1024" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="6" t="n">
+      <c r="C8" s="6">
         <v>1</v>
       </c>
       <c r="D8" s="7" t="s">
@@ -631,14 +856,14 @@
       </c>
       <c r="AMJ8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:1024" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="6" t="n">
+      <c r="C9" s="6">
         <v>2</v>
       </c>
       <c r="D9" s="7" t="s">
@@ -652,14 +877,14 @@
       </c>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:1024" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="6" t="n">
+      <c r="C10" s="6">
         <v>3</v>
       </c>
       <c r="D10" s="7" t="s">
@@ -673,12 +898,12 @@
       </c>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:1024" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="6" t="n">
+      <c r="C11" s="6">
         <v>1</v>
       </c>
       <c r="D11" s="7" t="s">
@@ -692,12 +917,12 @@
       </c>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:1024" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="6" t="n">
+      <c r="C12" s="6">
         <v>2</v>
       </c>
       <c r="D12" s="7" t="s">
@@ -711,12 +936,12 @@
       </c>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:1024" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
       <c r="B13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="6" t="n">
+      <c r="C13" s="6">
         <v>3</v>
       </c>
       <c r="D13" s="7" t="s">
@@ -728,7 +953,7 @@
       <c r="F13" s="7"/>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" s="3" customFormat="true" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:1024" s="3" customFormat="1" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
         <v>0</v>
       </c>
@@ -746,14 +971,14 @@
       </c>
       <c r="AMJ14" s="4"/>
     </row>
-    <row r="15" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:1024" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="6" t="n">
+      <c r="C15" s="6">
         <v>1</v>
       </c>
       <c r="D15" s="7" t="s">
@@ -767,14 +992,14 @@
       </c>
       <c r="AMJ15" s="1"/>
     </row>
-    <row r="16" s="6" customFormat="true" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:1024" s="6" customFormat="1" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="6" t="n">
+      <c r="C16" s="6">
         <v>2</v>
       </c>
       <c r="D16" s="7" t="s">
@@ -788,14 +1013,14 @@
       </c>
       <c r="AMJ16" s="1"/>
     </row>
-    <row r="17" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:1024" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="6" t="n">
+      <c r="C17" s="6">
         <v>3</v>
       </c>
       <c r="D17" s="7" t="s">
@@ -809,12 +1034,12 @@
       </c>
       <c r="AMJ17" s="1"/>
     </row>
-    <row r="18" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:1024" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="5"/>
       <c r="B18" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="6" t="n">
+      <c r="C18" s="6">
         <v>1</v>
       </c>
       <c r="D18" s="7" t="s">
@@ -834,12 +1059,12 @@
       </c>
       <c r="AMJ18" s="1"/>
     </row>
-    <row r="19" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:1024" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" s="5"/>
       <c r="B19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="6" t="n">
+      <c r="C19" s="6">
         <v>2</v>
       </c>
       <c r="D19" s="7" t="s">
@@ -859,12 +1084,12 @@
       </c>
       <c r="AMJ19" s="1"/>
     </row>
-    <row r="20" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:1024" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
       <c r="B20" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="6" t="n">
+      <c r="C20" s="6">
         <v>3</v>
       </c>
       <c r="D20" s="7" t="s">
@@ -884,7 +1109,7 @@
       </c>
       <c r="AMJ20" s="1"/>
     </row>
-    <row r="21" s="3" customFormat="true" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:1024" s="3" customFormat="1" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
         <v>0</v>
       </c>
@@ -902,14 +1127,14 @@
       </c>
       <c r="AMJ21" s="4"/>
     </row>
-    <row r="22" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:1024" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>41</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="6" t="n">
+      <c r="C22" s="6">
         <v>1</v>
       </c>
       <c r="D22" s="7" t="s">
@@ -924,14 +1149,14 @@
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:1024" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="6" t="n">
+      <c r="C23" s="6">
         <v>2</v>
       </c>
       <c r="D23" s="7" t="s">
@@ -946,14 +1171,14 @@
       <c r="G23" s="7"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:1024" ht="18" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>44</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="6" t="n">
+      <c r="C24" s="6">
         <v>3</v>
       </c>
       <c r="D24" s="7" t="s">
@@ -968,12 +1193,12 @@
       <c r="G24" s="7"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:1024" ht="18" x14ac:dyDescent="0.35">
       <c r="A25" s="5"/>
       <c r="B25" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="6" t="n">
+      <c r="C25" s="6">
         <v>1</v>
       </c>
       <c r="D25" s="7" t="s">
@@ -988,12 +1213,12 @@
       <c r="G25" s="7"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:1024" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="5"/>
       <c r="B26" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="6" t="n">
+      <c r="C26" s="6">
         <v>2</v>
       </c>
       <c r="D26" s="7" t="s">
@@ -1009,12 +1234,12 @@
       <c r="H26" s="7"/>
       <c r="AMJ26" s="1"/>
     </row>
-    <row r="27" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:1024" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" s="5"/>
       <c r="B27" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="6" t="n">
+      <c r="C27" s="6">
         <v>3</v>
       </c>
       <c r="D27" s="7" t="s">
@@ -1030,7 +1255,7 @@
       <c r="H27" s="7"/>
       <c r="AMJ27" s="1"/>
     </row>
-    <row r="28" s="3" customFormat="true" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:1024" s="3" customFormat="1" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A28" s="3" t="s">
         <v>0</v>
       </c>
@@ -1048,14 +1273,14 @@
       </c>
       <c r="AMJ28" s="4"/>
     </row>
-    <row r="29" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:1024" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>51</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="6" t="n">
+      <c r="C29" s="6">
         <v>1</v>
       </c>
       <c r="D29" s="7" t="s">
@@ -1070,14 +1295,14 @@
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
     </row>
-    <row r="30" s="6" customFormat="true" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:1024" s="6" customFormat="1" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A30" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="6" t="n">
+      <c r="C30" s="6">
         <v>2</v>
       </c>
       <c r="D30" s="7" t="s">
@@ -1092,14 +1317,14 @@
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
     </row>
-    <row r="31" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:1024" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>54</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="6" t="n">
+      <c r="C31" s="6">
         <v>3</v>
       </c>
       <c r="D31" s="7" t="s">
@@ -1114,12 +1339,12 @@
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
     </row>
-    <row r="32" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:1024" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A32" s="5"/>
       <c r="B32" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="6" t="n">
+      <c r="C32" s="6">
         <v>1</v>
       </c>
       <c r="D32" s="7" t="s">
@@ -1135,12 +1360,12 @@
       <c r="H32" s="7"/>
       <c r="AMJ32" s="1"/>
     </row>
-    <row r="33" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:1024" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A33" s="5"/>
       <c r="B33" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="6" t="n">
+      <c r="C33" s="6">
         <v>2</v>
       </c>
       <c r="D33" s="7" t="s">
@@ -1156,12 +1381,12 @@
       <c r="H33" s="7"/>
       <c r="AMJ33" s="1"/>
     </row>
-    <row r="34" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:1024" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A34" s="5"/>
       <c r="B34" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="6" t="n">
+      <c r="C34" s="6">
         <v>3</v>
       </c>
       <c r="D34" s="7" t="s">
@@ -1177,7 +1402,7 @@
       <c r="H34" s="7"/>
       <c r="AMJ34" s="1"/>
     </row>
-    <row r="35" s="3" customFormat="true" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:1024" s="3" customFormat="1" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A35" s="3" t="s">
         <v>0</v>
       </c>
@@ -1195,14 +1420,14 @@
       </c>
       <c r="AMJ35" s="4"/>
     </row>
-    <row r="36" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:1024" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>58</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C36" s="6" t="n">
+      <c r="C36" s="6">
         <v>1</v>
       </c>
       <c r="D36" s="7" t="s">
@@ -1217,14 +1442,14 @@
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
     </row>
-    <row r="37" s="6" customFormat="true" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:1024" s="6" customFormat="1" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A37" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C37" s="6" t="n">
+      <c r="C37" s="6">
         <v>2</v>
       </c>
       <c r="D37" s="7" t="s">
@@ -1239,14 +1464,14 @@
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
     </row>
-    <row r="38" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:1024" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="6" t="n">
+      <c r="C38" s="6">
         <v>3</v>
       </c>
       <c r="D38" s="7" t="s">
@@ -1262,12 +1487,12 @@
       <c r="H38" s="7"/>
       <c r="AMJ38" s="1"/>
     </row>
-    <row r="39" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:1024" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A39" s="5"/>
       <c r="B39" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="6" t="n">
+      <c r="C39" s="6">
         <v>1</v>
       </c>
       <c r="D39" s="7" t="s">
@@ -1287,12 +1512,12 @@
       </c>
       <c r="AMJ39" s="1"/>
     </row>
-    <row r="40" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:1024" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A40" s="5"/>
       <c r="B40" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C40" s="6" t="n">
+      <c r="C40" s="6">
         <v>2</v>
       </c>
       <c r="D40" s="7" t="s">
@@ -1312,12 +1537,12 @@
       </c>
       <c r="AMJ40" s="1"/>
     </row>
-    <row r="41" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:1024" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A41" s="5"/>
       <c r="B41" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="6" t="n">
+      <c r="C41" s="6">
         <v>3</v>
       </c>
       <c r="D41" s="7" t="s">
@@ -1333,7 +1558,7 @@
       <c r="H41" s="7"/>
       <c r="AMJ41" s="1"/>
     </row>
-    <row r="42" s="3" customFormat="true" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:1024" s="3" customFormat="1" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A42" s="3" t="s">
         <v>0</v>
       </c>
@@ -1351,14 +1576,14 @@
       </c>
       <c r="AMJ42" s="4"/>
     </row>
-    <row r="43" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:1024" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>65</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C43" s="6" t="n">
+      <c r="C43" s="6">
         <v>1</v>
       </c>
       <c r="D43" s="7" t="s">
@@ -1374,14 +1599,14 @@
       <c r="H43" s="7"/>
       <c r="I43" s="7"/>
     </row>
-    <row r="44" s="6" customFormat="true" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:1024" s="6" customFormat="1" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A44" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C44" s="6" t="n">
+      <c r="C44" s="6">
         <v>2</v>
       </c>
       <c r="D44" s="7" t="s">
@@ -1398,14 +1623,14 @@
       <c r="I44" s="7"/>
       <c r="AMJ44" s="1"/>
     </row>
-    <row r="45" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:1024" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
         <v>66</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C45" s="6" t="n">
+      <c r="C45" s="6">
         <v>3</v>
       </c>
       <c r="D45" s="7" t="s">
@@ -1422,12 +1647,12 @@
       <c r="I45" s="7"/>
       <c r="AMJ45" s="1"/>
     </row>
-    <row r="46" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:1024" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A46" s="5"/>
       <c r="B46" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C46" s="6" t="n">
+      <c r="C46" s="6">
         <v>1</v>
       </c>
       <c r="D46" s="7" t="s">
@@ -1444,12 +1669,12 @@
       <c r="I46" s="7"/>
       <c r="AMJ46" s="1"/>
     </row>
-    <row r="47" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:1024" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A47" s="5"/>
       <c r="B47" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C47" s="6" t="n">
+      <c r="C47" s="6">
         <v>2</v>
       </c>
       <c r="D47" s="7" t="s">
@@ -1466,12 +1691,12 @@
       <c r="I47" s="7"/>
       <c r="AMJ47" s="1"/>
     </row>
-    <row r="48" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:1024" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A48" s="5"/>
       <c r="B48" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C48" s="6" t="n">
+      <c r="C48" s="6">
         <v>3</v>
       </c>
       <c r="D48" s="7" t="s">
@@ -1488,12 +1713,12 @@
       <c r="I48" s="7"/>
       <c r="AMJ48" s="1"/>
     </row>
-    <row r="49" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:1024" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A49" s="5"/>
       <c r="B49" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C49" s="6" t="n">
+      <c r="C49" s="6">
         <v>4</v>
       </c>
       <c r="D49" s="7" t="s">
@@ -1511,10 +1736,9 @@
       <c r="AMJ49" s="1"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>